<commit_message>
working on detailed robot model
</commit_message>
<xml_diff>
--- a/design/parts calculations.xlsx
+++ b/design/parts calculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Part</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>8020 Joining plate 2rcx4</t>
-  </si>
-  <si>
     <t>tnuts</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>8020 carry handle 1xkc5</t>
   </si>
   <si>
-    <t>panel retainer 5jb82</t>
-  </si>
-  <si>
     <t>Grainger hinge for ramp 16u354</t>
   </si>
   <si>
@@ -91,6 +85,9 @@
   </si>
   <si>
     <t>Mcmaster wheels  29635T31</t>
+  </si>
+  <si>
+    <t>inside corner connector</t>
   </si>
 </sst>
 </file>
@@ -432,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +472,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -490,20 +487,20 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <f>C2*D2*E2</f>
-        <v>517.08000000000004</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="G2">
         <f>SUM(F:F)</f>
-        <v>1547.7494453701408</v>
+        <v>612.34944537014087</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -525,7 +522,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -544,12 +541,12 @@
         <v>29.08</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -558,22 +555,22 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>12.62</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <f>C5*D5*E5</f>
-        <v>201.92</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -582,20 +579,20 @@
         <v>1.06</v>
       </c>
       <c r="E6">
-        <f>E5*5+E3*3+E9*2+E10*4</f>
-        <v>170</v>
+        <f>E3*3+E9*2+10</f>
+        <v>20</v>
       </c>
       <c r="F6">
         <f>C6*D6*E6</f>
-        <v>180.20000000000002</v>
+        <v>21.200000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>0.9</v>
@@ -608,19 +605,19 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F29" si="0">C7*D7*E7</f>
+        <f t="shared" ref="F7:F28" si="0">C7*D7*E7</f>
         <v>172.91338582677164</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>0.4</v>
@@ -637,12 +634,12 @@
         <v>73.196850393700785</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -663,99 +660,83 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <f>0.38*0.88</f>
+        <v>0.33440000000000003</v>
       </c>
       <c r="D10">
-        <v>9.8699999999999992</v>
+        <f>127.5/(48*96*(0.0254^2))</f>
+        <v>42.887455566577806</v>
       </c>
       <c r="E10">
-        <f>4*5</f>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>197.39999999999998</v>
+        <v>57.366260565854482</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <f>0.38*0.88</f>
-        <v>0.33440000000000003</v>
+        <f>0.38*0.38</f>
+        <v>0.1444</v>
       </c>
       <c r="D11">
-        <f>127.5/(48*96*(0.0254^2))</f>
+        <f>D10</f>
         <v>42.887455566577806</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>57.366260565854482</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>6.192948583813835</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <f>0.38*0.38</f>
-        <v>0.1444</v>
-      </c>
-      <c r="D12">
-        <f>D11</f>
-        <v>42.887455566577806</v>
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>15.11</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>6.192948583813835</v>
+        <v>30.22</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>15.11</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>30.22</v>
+        <f>C13*D13*E12</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F14">
-        <f>C14*D14*E13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -839,12 +820,6 @@
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>